<commit_message>
Better dir names. Recent data.
</commit_message>
<xml_diff>
--- a/RMR/RMR.xlsx
+++ b/RMR/RMR.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\lucent\health-data\RMR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{251F6BA4-9EA9-4975-B773-3C0648F1A44C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA70F36-8925-4615-8BF1-A48B32CBE123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11370" yWindow="3930" windowWidth="20745" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40" yWindow="2760" windowWidth="16500" windowHeight="12910" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,12 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Date</t>
   </si>
   <si>
     <t>RMR</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Cosmed</t>
   </si>
 </sst>
 </file>
@@ -38,7 +44,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -71,7 +77,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A22"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -363,179 +369,191 @@
     <col min="1" max="1" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>40663</v>
       </c>
       <c r="B2">
         <v>2415</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>41032</v>
       </c>
       <c r="B3">
         <v>1956</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42399</v>
       </c>
       <c r="B4">
         <v>1700</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>44686</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1981</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>44687</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>1989</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>44690</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2283</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>44691</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>2002</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>44700</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>2247</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>44701</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>2292</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>44714</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>2034</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>44736</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>2024</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>44878</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>1976</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>44879</v>
       </c>
-      <c r="B14">
+      <c r="B15">
         <v>1997</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>44884</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>1844</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>44891</v>
-      </c>
-      <c r="B16">
-        <v>1776</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
-        <v>44962</v>
+        <v>44891</v>
       </c>
       <c r="B17">
-        <v>1935</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
-        <v>44964</v>
+        <v>44962</v>
       </c>
       <c r="B18">
-        <v>1791</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
-        <v>44967</v>
+        <v>44964</v>
       </c>
       <c r="B19">
-        <v>1918</v>
+        <v>1791</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
-        <v>45067</v>
+        <v>44967</v>
       </c>
       <c r="B20">
-        <v>2022</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
-        <v>45095</v>
+        <v>45067</v>
       </c>
       <c r="B21">
-        <v>2241</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
+        <v>45095</v>
+      </c>
+      <c r="B22">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>45096</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>1884</v>
       </c>
     </row>

</xml_diff>